<commit_message>
:bug: fix: Ajustes para melhor performance
</commit_message>
<xml_diff>
--- a/Selenium/produto_scrap.xlsx
+++ b/Selenium/produto_scrap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Perilo\OneDrive\Documentos\Python\Estoque\Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41F3B03-CBF3-4265-95D0-9E5A41DAD206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F1E5F9-6DC4-4967-89B3-37545E0FC6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C12CF50E-6C77-46B7-8DF1-01ECE73E54EB}"/>
   </bookViews>
@@ -51,6 +51,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -80,9 +83,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -100,6 +106,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -119,12 +126,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FFDD24EF-CCEE-49B6-9CCA-5CE847B1EB9B}" name="Tabela2" displayName="Tabela2" ref="A1:C1048576" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FFDD24EF-CCEE-49B6-9CCA-5CE847B1EB9B}" name="Tabela2" displayName="Tabela2" ref="A1:C1048576" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
   <autoFilter ref="A1:C1048576" xr:uid="{FFDD24EF-CCEE-49B6-9CCA-5CE847B1EB9B}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9BA31AFF-2E2C-4049-A1C1-3DC86DD84871}" name="Produto" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{59E6AC8B-744E-4A77-9BD7-ADE7D5AE7C30}" name="Preço" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{A0FBA922-CFED-4379-A639-71EE9441A350}" name="Imagem" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{9BA31AFF-2E2C-4049-A1C1-3DC86DD84871}" name="Produto" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{59E6AC8B-744E-4A77-9BD7-ADE7D5AE7C30}" name="Preço" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{A0FBA922-CFED-4379-A639-71EE9441A350}" name="Imagem" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -450,12 +457,13 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="40.7109375" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -464,7 +472,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -486,10 +494,10 @@
     <row r="14" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">

</xml_diff>